<commit_message>
continue on constructing final_df
</commit_message>
<xml_diff>
--- a/DownloadDataForDK/ModelData/Final_Dataset/Fundamentals.xlsx
+++ b/DownloadDataForDK/ModelData/Final_Dataset/Fundamentals.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,16 @@
           <t>EmissionIntensity/EmissionIntensity</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>EmissionTax/EmissionType</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>EmissionTax/EmissionTax</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -482,6 +492,14 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>CO2</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>24.64</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -505,6 +523,8 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -528,6 +548,8 @@
       <c r="E4" t="n">
         <v>0.3397319999728214</v>
       </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -551,6 +573,8 @@
       <c r="E5" t="n">
         <v>0.205199999983584</v>
       </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -574,6 +598,8 @@
       <c r="E6" t="n">
         <v>0.2759219999779262</v>
       </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -597,6 +623,8 @@
       <c r="E7" t="n">
         <v>0.15299999998776</v>
       </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>